<commit_message>
commit the df_subaru after modifications: correct model B9 Tribeca (2006, 2007) and Tribeca (up to 2008)
</commit_message>
<xml_diff>
--- a/dataframe_each_make_xlsx_file/df_subaru_updated.xlsx
+++ b/dataframe_each_make_xlsx_file/df_subaru_updated.xlsx
@@ -837,8 +837,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>B9 Tribeca (2006 – 2007)
-Tribeca (2008 – onward)</t>
+          <t>Tribeca</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -907,8 +906,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>B9 Tribeca (2006 – 2007)
-Tribeca (2008 – onward)</t>
+          <t>Tribeca</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1092,8 +1090,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>B9 Tribeca (2006 – 2007)
-Tribeca (2008 – onward)</t>
+          <t>Tribeca</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1139,8 +1136,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>B9 Tribeca (2006 – 2007)
-Tribeca (2008 – onward)</t>
+          <t>Tribeca</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1255,8 +1251,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>B9 Tribeca (2006 – 2007)
-Tribeca (2008 – onward)</t>
+          <t>Tribeca</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1440,8 +1435,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>B9 Tribeca (2006 – 2007)
-Tribeca (2008 – onward)</t>
+          <t>Tribeca</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1487,8 +1481,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>B9 Tribeca (2006 – 2007)
-Tribeca (2008 – onward)</t>
+          <t>Tribeca</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1626,8 +1619,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>B9 Tribeca (2006 – 2007)
-Tribeca (2008 – onward)</t>
+          <t>Tribeca</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">

</xml_diff>